<commit_message>
feat: add b2-b5.xlsx again
</commit_message>
<xml_diff>
--- a/data/raw/raw_boms.xlsx
+++ b/data/raw/raw_boms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6127F36B-5301-4A38-8AF4-929543471649}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA546D53-7A18-48C1-BBE9-E90F22590080}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="191">
   <si>
     <t>Building Type</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Exterior Walls</t>
   </si>
   <si>
-    <t>Curtain wall, steel spandrel</t>
-  </si>
-  <si>
     <t>Glazing</t>
   </si>
   <si>
@@ -260,18 +257,12 @@
     <t>Paint, interior acrylic latex</t>
   </si>
   <si>
-    <t>Curtain wall, alu spandrel</t>
-  </si>
-  <si>
     <t>Aluminum Curtain Wall System</t>
   </si>
   <si>
     <t>Aluminum curtain wall system, YKK AP - EPD</t>
   </si>
   <si>
-    <t>MV - Brick</t>
-  </si>
-  <si>
     <t>Brick</t>
   </si>
   <si>
@@ -317,9 +308,6 @@
     <t>Gypsum wall board</t>
   </si>
   <si>
-    <t>MV - Granite</t>
-  </si>
-  <si>
     <t>4" granite veneer</t>
   </si>
   <si>
@@ -332,9 +320,6 @@
     <t>Mortar type S</t>
   </si>
   <si>
-    <t>Insulated Metal Panel</t>
-  </si>
-  <si>
     <t>Exterior finish + insulation</t>
   </si>
   <si>
@@ -377,9 +362,6 @@
     <t>AVB Membrane</t>
   </si>
   <si>
-    <t>Rainscreen, GFRC</t>
-  </si>
-  <si>
     <t>Glass Fiber Reinforced Concrete (GFRC) Panel</t>
   </si>
   <si>
@@ -392,9 +374,6 @@
     <t>4.5" Mineral Wool insulation</t>
   </si>
   <si>
-    <t>Rainscreen, Thin brick</t>
-  </si>
-  <si>
     <t>3/4" Brick</t>
   </si>
   <si>
@@ -425,9 +404,6 @@
     <t>3.5" Mineral Wool insulation</t>
   </si>
   <si>
-    <t>Rainscreen, Wood</t>
-  </si>
-  <si>
     <t>6" x 1' Tulipwood/Poplar Lumber</t>
   </si>
   <si>
@@ -446,9 +422,6 @@
     <t>Aluminum extrusion, AEC - EPD</t>
   </si>
   <si>
-    <t>Rainscreen, Formed Steel Panel</t>
-  </si>
-  <si>
     <t>Formed Steel Sheet</t>
   </si>
   <si>
@@ -491,9 +464,6 @@
     <t>Viracon triple pane IGU, 1-5/16" Clear Insulating Low-E Laminated  Glass Unit with a ½” VTS Airspace  and Both Lites Heat Treated</t>
   </si>
   <si>
-    <t>Operable window</t>
-  </si>
-  <si>
     <t>21-02 30 10</t>
   </si>
   <si>
@@ -618,6 +588,15 @@
   </si>
   <si>
     <t>Glue laminated timber (Glulam), AWC - EPD</t>
+  </si>
+  <si>
+    <t>Curtain wall: alu spandrel</t>
+  </si>
+  <si>
+    <t>Glazing: double pane IGU</t>
+  </si>
+  <si>
+    <t>Glazing: triple pane IGU</t>
   </si>
 </sst>
 </file>
@@ -1089,8 +1068,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1164,7 +1143,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>17</v>
@@ -1202,7 +1181,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>17</v>
@@ -1240,7 +1219,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>24</v>
@@ -1278,7 +1257,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>24</v>
@@ -1316,7 +1295,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>26</v>
@@ -1354,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>26</v>
@@ -1392,7 +1371,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
@@ -1430,7 +1409,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>34</v>
@@ -1439,10 +1418,10 @@
         <v>38</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="K9" s="10">
         <v>132267</v>
@@ -1468,7 +1447,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>34</v>
@@ -1506,7 +1485,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>39</v>
@@ -1518,7 +1497,7 @@
         <v>41</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="K11" s="10">
         <v>217730</v>
@@ -1544,7 +1523,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>42</v>
@@ -1556,7 +1535,7 @@
         <v>41</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="K12" s="10">
         <v>89824</v>
@@ -1582,7 +1561,7 @@
         <v>33</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>43</v>
@@ -1594,7 +1573,7 @@
         <v>41</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="K13" s="10">
         <v>44674</v>
@@ -1620,7 +1599,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>44</v>
@@ -1658,7 +1637,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>44</v>
@@ -1696,7 +1675,7 @@
         <v>16</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>17</v>
@@ -1734,7 +1713,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>17</v>
@@ -1772,7 +1751,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>24</v>
@@ -1810,7 +1789,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>24</v>
@@ -1848,7 +1827,7 @@
         <v>16</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>26</v>
@@ -1886,7 +1865,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>26</v>
@@ -1924,7 +1903,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>34</v>
@@ -1962,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>34</v>
@@ -2000,7 +1979,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>43</v>
@@ -2038,7 +2017,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>43</v>
@@ -2076,7 +2055,7 @@
         <v>33</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>44</v>
@@ -2114,7 +2093,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>44</v>
@@ -2152,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>17</v>
@@ -2190,7 +2169,7 @@
         <v>16</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>17</v>
@@ -2228,7 +2207,7 @@
         <v>16</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>24</v>
@@ -2266,7 +2245,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>24</v>
@@ -2304,7 +2283,7 @@
         <v>16</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>26</v>
@@ -2342,7 +2321,7 @@
         <v>16</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>26</v>
@@ -2380,7 +2359,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>34</v>
@@ -2418,7 +2397,7 @@
         <v>33</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>34</v>
@@ -2456,7 +2435,7 @@
         <v>33</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>34</v>
@@ -2494,7 +2473,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>39</v>
@@ -2506,7 +2485,7 @@
         <v>55</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K37" s="10">
         <v>54158</v>
@@ -2532,7 +2511,7 @@
         <v>33</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>42</v>
@@ -2544,7 +2523,7 @@
         <v>55</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K38" s="10">
         <v>227907</v>
@@ -2570,7 +2549,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>43</v>
@@ -2582,7 +2561,7 @@
         <v>55</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K39" s="10">
         <v>136704</v>
@@ -2608,7 +2587,7 @@
         <v>33</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>44</v>
@@ -2646,7 +2625,7 @@
         <v>33</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>44</v>
@@ -2746,25 +2725,25 @@
         <v>58</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H2" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>63</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>64</v>
       </c>
       <c r="K2" s="27">
         <v>31445</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2784,25 +2763,25 @@
         <v>58</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H3" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I3" s="25" t="s">
-        <v>66</v>
-      </c>
       <c r="J3" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="27">
         <v>479</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2822,25 +2801,25 @@
         <v>58</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H4" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="J4" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="K4" s="27">
         <v>10981</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2860,25 +2839,25 @@
         <v>58</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H5" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="J5" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J5" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K5" s="27">
         <v>14975</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2898,25 +2877,25 @@
         <v>58</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="J6" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K6" s="27">
         <v>30644</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2936,25 +2915,25 @@
         <v>58</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K7" s="27">
         <v>509</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2974,25 +2953,25 @@
         <v>58</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K8" s="27">
         <v>10917</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3012,25 +2991,25 @@
         <v>58</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H9" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="J9" s="25" t="s">
         <v>68</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>69</v>
       </c>
       <c r="K9" s="27">
         <v>10806</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3050,25 +3029,25 @@
         <v>58</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H10" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="J10" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K10" s="27">
         <v>14975</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3088,25 +3067,25 @@
         <v>58</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H11" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="J11" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K11" s="27">
         <v>30644</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3126,25 +3105,25 @@
         <v>58</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K12" s="27">
         <v>509</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3164,25 +3143,25 @@
         <v>58</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K13" s="27">
         <v>360492</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3202,25 +3181,25 @@
         <v>58</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K14" s="27">
         <v>57846</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3240,25 +3219,25 @@
         <v>58</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K15" s="27">
         <v>12117</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3278,25 +3257,25 @@
         <v>58</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K16" s="27">
         <v>9412</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -3316,25 +3295,25 @@
         <v>58</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K17" s="27">
         <v>6719</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -3354,25 +3333,25 @@
         <v>58</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J18" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K18" s="27">
         <v>30261</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -3392,25 +3371,25 @@
         <v>58</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J19" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K19" s="27">
         <v>14975</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -3430,25 +3409,25 @@
         <v>58</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J20" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K20" s="27">
         <v>30644</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -3468,25 +3447,25 @@
         <v>58</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K21" s="27">
         <v>509</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -3506,25 +3485,25 @@
         <v>58</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H22" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="J22" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K22" s="27">
         <v>624440</v>
       </c>
       <c r="L22" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -3544,25 +3523,25 @@
         <v>58</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H23" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K23" s="27">
         <v>22658</v>
       </c>
       <c r="L23" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3582,25 +3561,25 @@
         <v>58</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J24" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K24" s="27">
         <v>12117</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -3620,25 +3599,25 @@
         <v>58</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J25" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K25" s="27">
         <v>9412</v>
       </c>
       <c r="L25" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -3658,25 +3637,25 @@
         <v>58</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H26" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I26" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J26" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K26" s="27">
         <v>6719</v>
       </c>
       <c r="L26" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -3696,25 +3675,25 @@
         <v>58</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K27" s="27">
         <v>30261</v>
       </c>
       <c r="L27" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -3734,25 +3713,25 @@
         <v>58</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H28" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K28" s="27">
         <v>14975</v>
       </c>
       <c r="L28" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -3772,25 +3751,25 @@
         <v>58</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H29" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K29" s="27">
         <v>30644</v>
       </c>
       <c r="L29" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -3810,25 +3789,25 @@
         <v>58</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I30" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J30" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K30" s="27">
         <v>509</v>
       </c>
       <c r="L30" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -3848,25 +3827,25 @@
         <v>58</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J31" s="43" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="K31" s="27">
         <v>29658</v>
       </c>
       <c r="L31" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -3886,25 +3865,25 @@
         <v>58</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H32" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J32" s="25" t="s">
         <v>65</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="J32" s="25" t="s">
-        <v>66</v>
       </c>
       <c r="K32" s="27">
         <v>753</v>
       </c>
       <c r="L32" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -3924,25 +3903,25 @@
         <v>58</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H33" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J33" s="25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K33" s="27">
         <v>2077</v>
       </c>
       <c r="L33" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -3962,25 +3941,25 @@
         <v>58</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H34" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="25" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J34" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K34" s="27">
         <v>14975</v>
       </c>
       <c r="L34" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -4000,25 +3979,25 @@
         <v>58</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H35" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K35" s="27">
         <v>30644</v>
       </c>
       <c r="L35" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -4038,25 +4017,25 @@
         <v>58</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H36" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I36" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J36" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K36" s="27">
         <v>509</v>
       </c>
       <c r="L36" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -4076,25 +4055,25 @@
         <v>58</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G37" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H37" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K37" s="27">
         <v>1564</v>
       </c>
       <c r="L37" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -4114,25 +4093,25 @@
         <v>58</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G38" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J38" s="25" t="s">
         <v>110</v>
-      </c>
-      <c r="H38" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="I38" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="J38" s="25" t="s">
-        <v>115</v>
       </c>
       <c r="K38" s="27">
         <v>3969</v>
       </c>
       <c r="L38" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -4152,25 +4131,25 @@
         <v>58</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G39" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H39" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I39" s="25" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K39" s="27">
         <v>6719</v>
       </c>
       <c r="L39" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -4190,25 +4169,25 @@
         <v>58</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H40" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I40" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K40" s="27">
         <v>30261</v>
       </c>
       <c r="L40" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -4228,25 +4207,25 @@
         <v>58</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G41" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H41" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I41" s="25" t="s">
+      <c r="J41" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J41" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K41" s="27">
         <v>14975</v>
       </c>
       <c r="L41" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -4266,25 +4245,25 @@
         <v>58</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H42" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="J42" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J42" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K42" s="27">
         <v>30644</v>
       </c>
       <c r="L42" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -4304,25 +4283,25 @@
         <v>58</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="G43" s="31" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H43" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I43" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J43" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J43" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K43" s="27">
         <v>509</v>
       </c>
       <c r="L43" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -4342,25 +4321,25 @@
         <v>58</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H44" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I44" s="25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K44" s="27">
         <v>170263</v>
       </c>
       <c r="L44" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -4380,25 +4359,25 @@
         <v>58</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H45" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I45" s="25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K45" s="27">
         <v>97036</v>
       </c>
       <c r="L45" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -4418,25 +4397,25 @@
         <v>58</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J46" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K46" s="27">
         <v>10632</v>
       </c>
       <c r="L46" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -4456,25 +4435,25 @@
         <v>58</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H47" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I47" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J47" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K47" s="27">
         <v>6719</v>
       </c>
       <c r="L47" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -4494,25 +4473,25 @@
         <v>58</v>
       </c>
       <c r="F48" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I48" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J48" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K48" s="27">
         <v>30261</v>
       </c>
       <c r="L48" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -4532,25 +4511,25 @@
         <v>58</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H49" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I49" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I49" s="25" t="s">
+      <c r="J49" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J49" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K49" s="27">
         <v>14975</v>
       </c>
       <c r="L49" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -4570,25 +4549,25 @@
         <v>58</v>
       </c>
       <c r="F50" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H50" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I50" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I50" s="25" t="s">
+      <c r="J50" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J50" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K50" s="27">
         <v>30644</v>
       </c>
       <c r="L50" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -4608,25 +4587,25 @@
         <v>58</v>
       </c>
       <c r="F51" s="41" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="G51" s="32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="H51" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I51" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J51" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J51" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K51" s="27">
         <v>509</v>
       </c>
       <c r="L51" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -4646,25 +4625,25 @@
         <v>58</v>
       </c>
       <c r="F52" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H52" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I52" s="25" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="K52" s="27">
         <v>74168</v>
       </c>
       <c r="L52" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -4684,25 +4663,25 @@
         <v>58</v>
       </c>
       <c r="F53" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I53" s="25" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="J53" s="25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="K53" s="27">
         <v>11329</v>
       </c>
       <c r="L53" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -4722,25 +4701,25 @@
         <v>58</v>
       </c>
       <c r="F54" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H54" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I54" s="25" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="J54" s="25" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="K54" s="27">
         <v>425</v>
       </c>
       <c r="L54" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -4760,25 +4739,25 @@
         <v>58</v>
       </c>
       <c r="F55" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I55" s="25" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J55" s="41" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="K55" s="27">
         <v>16759</v>
       </c>
       <c r="L55" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -4798,25 +4777,25 @@
         <v>58</v>
       </c>
       <c r="F56" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H56" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I56" s="25" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J56" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K56" s="27">
         <v>4039</v>
       </c>
       <c r="L56" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -4836,25 +4815,25 @@
         <v>58</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I57" s="25" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J57" s="25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="K57" s="27">
         <v>96</v>
       </c>
       <c r="L57" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -4874,25 +4853,25 @@
         <v>58</v>
       </c>
       <c r="F58" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H58" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I58" s="25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J58" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K58" s="27">
         <v>8366</v>
       </c>
       <c r="L58" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -4912,25 +4891,25 @@
         <v>58</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H59" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I59" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J59" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K59" s="27">
         <v>6719</v>
       </c>
       <c r="L59" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -4950,25 +4929,25 @@
         <v>58</v>
       </c>
       <c r="F60" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H60" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I60" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J60" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K60" s="27">
         <v>30261</v>
       </c>
       <c r="L60" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -4988,25 +4967,25 @@
         <v>58</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G61" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H61" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I61" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I61" s="25" t="s">
+      <c r="J61" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J61" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K61" s="27">
         <v>14975</v>
       </c>
       <c r="L61" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -5026,25 +5005,25 @@
         <v>58</v>
       </c>
       <c r="F62" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G62" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H62" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I62" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I62" s="25" t="s">
+      <c r="J62" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J62" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K62" s="27">
         <v>30644</v>
       </c>
       <c r="L62" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -5064,25 +5043,25 @@
         <v>58</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="H63" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I63" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J63" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J63" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K63" s="27">
         <v>509</v>
       </c>
       <c r="L63" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -5102,25 +5081,25 @@
         <v>58</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H64" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I64" s="25" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="J64" s="25" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="K64" s="27">
         <v>25945</v>
       </c>
       <c r="L64" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -5140,25 +5119,25 @@
         <v>58</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H65" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I65" s="25" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J65" s="25" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K65" s="27">
         <v>208</v>
       </c>
       <c r="L65" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -5178,25 +5157,25 @@
         <v>58</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H66" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I66" s="25" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J66" s="25" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K66" s="27">
         <v>2717</v>
       </c>
       <c r="L66" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -5216,25 +5195,25 @@
         <v>58</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I67" s="25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J67" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K67" s="27">
         <v>4039</v>
       </c>
       <c r="L67" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -5254,25 +5233,25 @@
         <v>58</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H68" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I68" s="25" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J68" s="25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="K68" s="27">
         <v>96</v>
       </c>
       <c r="L68" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -5292,25 +5271,25 @@
         <v>58</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H69" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I69" s="25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J69" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K69" s="27">
         <v>8366</v>
       </c>
       <c r="L69" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -5330,25 +5309,25 @@
         <v>58</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H70" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I70" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J70" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K70" s="27">
         <v>6719</v>
       </c>
       <c r="L70" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -5368,25 +5347,25 @@
         <v>58</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H71" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I71" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J71" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K71" s="27">
         <v>30261</v>
       </c>
       <c r="L71" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -5406,25 +5385,25 @@
         <v>58</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H72" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I72" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I72" s="25" t="s">
+      <c r="J72" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J72" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K72" s="27">
         <v>14975</v>
       </c>
       <c r="L72" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -5444,25 +5423,25 @@
         <v>58</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G73" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H73" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I73" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I73" s="25" t="s">
+      <c r="J73" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J73" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K73" s="27">
         <v>30644</v>
       </c>
       <c r="L73" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -5482,25 +5461,25 @@
         <v>58</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G74" s="34" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="H74" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I74" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J74" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J74" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K74" s="27">
         <v>509</v>
       </c>
       <c r="L74" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -5520,25 +5499,25 @@
         <v>58</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G75" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H75" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I75" s="25" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J75" s="25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="K75" s="27">
         <v>11388</v>
       </c>
       <c r="L75" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -5558,25 +5537,25 @@
         <v>58</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G76" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H76" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I76" s="25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="J76" s="25" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="K76" s="27">
         <v>661</v>
       </c>
       <c r="L76" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -5596,25 +5575,25 @@
         <v>58</v>
       </c>
       <c r="F77" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G77" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H77" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I77" s="25" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="J77" s="25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K77" s="27">
         <v>323</v>
       </c>
       <c r="L77" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -5634,25 +5613,25 @@
         <v>58</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G78" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H78" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I78" s="25" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J78" s="25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K78" s="27">
         <v>4039</v>
       </c>
       <c r="L78" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -5672,25 +5651,25 @@
         <v>58</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G79" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H79" s="25" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="J79" s="25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="K79" s="27">
         <v>96</v>
       </c>
       <c r="L79" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -5710,25 +5689,25 @@
         <v>58</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G80" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H80" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I80" s="25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="J80" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K80" s="27">
         <v>8366</v>
       </c>
       <c r="L80" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5748,25 +5727,25 @@
         <v>58</v>
       </c>
       <c r="F81" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G81" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H81" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I81" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K81" s="27">
         <v>6719</v>
       </c>
       <c r="L81" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -5786,25 +5765,25 @@
         <v>58</v>
       </c>
       <c r="F82" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G82" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H82" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I82" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J82" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="K82" s="27">
         <v>30261</v>
       </c>
       <c r="L82" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -5824,25 +5803,25 @@
         <v>58</v>
       </c>
       <c r="F83" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G83" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H83" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I83" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="I83" s="25" t="s">
+      <c r="J83" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="J83" s="25" t="s">
-        <v>72</v>
       </c>
       <c r="K83" s="27">
         <v>14975</v>
       </c>
       <c r="L83" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -5862,25 +5841,25 @@
         <v>58</v>
       </c>
       <c r="F84" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G84" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H84" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I84" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="I84" s="25" t="s">
+      <c r="J84" s="25" t="s">
         <v>74</v>
-      </c>
-      <c r="J84" s="25" t="s">
-        <v>75</v>
       </c>
       <c r="K84" s="27">
         <v>30644</v>
       </c>
       <c r="L84" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -5900,25 +5879,25 @@
         <v>58</v>
       </c>
       <c r="F85" s="41" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="G85" s="35" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="H85" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I85" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J85" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="J85" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="K85" s="27">
         <v>509</v>
       </c>
       <c r="L85" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -8693,7 +8672,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>31</v>
@@ -8702,28 +8681,28 @@
         <v>57</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="J2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="K2" s="27">
         <v>35343</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75">
@@ -8731,7 +8710,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>31</v>
@@ -8740,28 +8719,28 @@
         <v>57</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="K3" s="27">
         <v>54275</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75">
@@ -11544,31 +11523,31 @@
         <v>12</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="K2" s="27">
         <v>10829</v>
@@ -11579,31 +11558,31 @@
         <v>12</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="K3" s="27">
         <v>9755</v>
@@ -14319,10 +14298,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855F4CF-4650-45D4-87F0-B29B2A97A803}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14335,7 +14314,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -14404,7 +14383,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -14412,7 +14391,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="B11">
         <v>35</v>
@@ -14420,7 +14399,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -14428,7 +14407,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
       <c r="B13">
         <v>35</v>
@@ -14436,7 +14415,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -14444,7 +14423,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B15">
         <v>35</v>
@@ -14452,7 +14431,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>174</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -14460,7 +14439,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="B17">
         <v>35</v>
@@ -14468,7 +14447,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="B18">
         <v>35</v>
@@ -14476,7 +14455,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="B19">
         <v>35</v>
@@ -14484,7 +14463,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -14492,25 +14471,17 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="B21">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>155</v>
+      <c r="A22" s="40" t="s">
+        <v>149</v>
       </c>
       <c r="B22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="B23">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add replacement impacts to impact calculator
</commit_message>
<xml_diff>
--- a/data/raw/raw_boms.xlsx
+++ b/data/raw/raw_boms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA546D53-7A18-48C1-BBE9-E90F22590080}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5A8D98-13CA-4F57-9805-EF6D0E29D53E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6870" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="189">
   <si>
     <t>Building Type</t>
   </si>
@@ -446,16 +446,10 @@
     <t>Exterior Windows</t>
   </si>
   <si>
-    <t>Glazing, double pane IGU</t>
-  </si>
-  <si>
     <t>Double pane IGU</t>
   </si>
   <si>
     <t>Viracon IGU, 1” Clear Insulating Low-E Glass Unit with a  ½” VTS Airspace and Both Lites Fully Tempered  and Heat Soak Tested</t>
-  </si>
-  <si>
-    <t>Glazing, triple pane IGU</t>
   </si>
   <si>
     <t>Triple pane IGU</t>
@@ -1143,7 +1137,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>17</v>
@@ -1181,7 +1175,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>17</v>
@@ -1219,7 +1213,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>24</v>
@@ -1257,7 +1251,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>24</v>
@@ -1295,7 +1289,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>26</v>
@@ -1333,7 +1327,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>26</v>
@@ -1371,7 +1365,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
@@ -1409,7 +1403,7 @@
         <v>33</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>34</v>
@@ -1418,10 +1412,10 @@
         <v>38</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K9" s="10">
         <v>132267</v>
@@ -1447,7 +1441,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>34</v>
@@ -1485,7 +1479,7 @@
         <v>33</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>39</v>
@@ -1497,7 +1491,7 @@
         <v>41</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K11" s="10">
         <v>217730</v>
@@ -1523,7 +1517,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>42</v>
@@ -1535,7 +1529,7 @@
         <v>41</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K12" s="10">
         <v>89824</v>
@@ -1561,7 +1555,7 @@
         <v>33</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>43</v>
@@ -1573,7 +1567,7 @@
         <v>41</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K13" s="10">
         <v>44674</v>
@@ -1599,7 +1593,7 @@
         <v>33</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>44</v>
@@ -1637,7 +1631,7 @@
         <v>33</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>44</v>
@@ -1675,7 +1669,7 @@
         <v>16</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>17</v>
@@ -1713,7 +1707,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>17</v>
@@ -1751,7 +1745,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>24</v>
@@ -1789,7 +1783,7 @@
         <v>16</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>24</v>
@@ -1827,7 +1821,7 @@
         <v>16</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>26</v>
@@ -1865,7 +1859,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>26</v>
@@ -1903,7 +1897,7 @@
         <v>33</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G22" s="13" t="s">
         <v>34</v>
@@ -1941,7 +1935,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>34</v>
@@ -1979,7 +1973,7 @@
         <v>33</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>43</v>
@@ -2017,7 +2011,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>43</v>
@@ -2055,7 +2049,7 @@
         <v>33</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>44</v>
@@ -2093,7 +2087,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>44</v>
@@ -2131,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G28" s="16" t="s">
         <v>17</v>
@@ -2169,7 +2163,7 @@
         <v>16</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>17</v>
@@ -2207,7 +2201,7 @@
         <v>16</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>24</v>
@@ -2245,7 +2239,7 @@
         <v>16</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>24</v>
@@ -2283,7 +2277,7 @@
         <v>16</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G32" s="16" t="s">
         <v>26</v>
@@ -2321,7 +2315,7 @@
         <v>16</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>26</v>
@@ -2359,7 +2353,7 @@
         <v>33</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G34" s="16" t="s">
         <v>34</v>
@@ -2397,7 +2391,7 @@
         <v>33</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>34</v>
@@ -2435,7 +2429,7 @@
         <v>33</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>34</v>
@@ -2473,7 +2467,7 @@
         <v>33</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>39</v>
@@ -2485,7 +2479,7 @@
         <v>55</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K37" s="10">
         <v>54158</v>
@@ -2511,7 +2505,7 @@
         <v>33</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>42</v>
@@ -2523,7 +2517,7 @@
         <v>55</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K38" s="10">
         <v>227907</v>
@@ -2549,7 +2543,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>43</v>
@@ -2561,7 +2555,7 @@
         <v>55</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K39" s="10">
         <v>136704</v>
@@ -2587,7 +2581,7 @@
         <v>33</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>44</v>
@@ -2625,7 +2619,7 @@
         <v>33</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>44</v>
@@ -2725,10 +2719,10 @@
         <v>58</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>61</v>
@@ -2763,10 +2757,10 @@
         <v>58</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>64</v>
@@ -2801,10 +2795,10 @@
         <v>58</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>66</v>
@@ -2839,10 +2833,10 @@
         <v>58</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>69</v>
@@ -2877,10 +2871,10 @@
         <v>58</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>72</v>
@@ -2915,10 +2909,10 @@
         <v>58</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>72</v>
@@ -2953,10 +2947,10 @@
         <v>58</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H8" s="25" t="s">
         <v>61</v>
@@ -2991,10 +2985,10 @@
         <v>58</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>66</v>
@@ -3029,10 +3023,10 @@
         <v>58</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>69</v>
@@ -3067,10 +3061,10 @@
         <v>58</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>72</v>
@@ -3105,10 +3099,10 @@
         <v>58</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H12" s="25" t="s">
         <v>72</v>
@@ -3143,10 +3137,10 @@
         <v>58</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H13" s="25" t="s">
         <v>64</v>
@@ -3181,10 +3175,10 @@
         <v>58</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H14" s="25" t="s">
         <v>64</v>
@@ -3219,10 +3213,10 @@
         <v>58</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H15" s="25" t="s">
         <v>83</v>
@@ -3257,10 +3251,10 @@
         <v>58</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H16" s="25" t="s">
         <v>66</v>
@@ -3295,10 +3289,10 @@
         <v>58</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G17" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H17" s="25" t="s">
         <v>87</v>
@@ -3333,10 +3327,10 @@
         <v>58</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>69</v>
@@ -3371,10 +3365,10 @@
         <v>58</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H19" s="25" t="s">
         <v>69</v>
@@ -3409,10 +3403,10 @@
         <v>58</v>
       </c>
       <c r="F20" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H20" s="25" t="s">
         <v>72</v>
@@ -3447,10 +3441,10 @@
         <v>58</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H21" s="25" t="s">
         <v>72</v>
@@ -3485,10 +3479,10 @@
         <v>58</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H22" s="25" t="s">
         <v>64</v>
@@ -3523,10 +3517,10 @@
         <v>58</v>
       </c>
       <c r="F23" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H23" s="25" t="s">
         <v>64</v>
@@ -3561,10 +3555,10 @@
         <v>58</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H24" s="25" t="s">
         <v>83</v>
@@ -3599,10 +3593,10 @@
         <v>58</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>66</v>
@@ -3637,10 +3631,10 @@
         <v>58</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H26" s="25" t="s">
         <v>87</v>
@@ -3675,10 +3669,10 @@
         <v>58</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H27" s="25" t="s">
         <v>69</v>
@@ -3713,10 +3707,10 @@
         <v>58</v>
       </c>
       <c r="F28" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G28" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H28" s="25" t="s">
         <v>69</v>
@@ -3751,10 +3745,10 @@
         <v>58</v>
       </c>
       <c r="F29" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H29" s="25" t="s">
         <v>72</v>
@@ -3789,10 +3783,10 @@
         <v>58</v>
       </c>
       <c r="F30" s="41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>72</v>
@@ -3827,10 +3821,10 @@
         <v>58</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G31" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H31" s="25" t="s">
         <v>98</v>
@@ -3839,7 +3833,7 @@
         <v>99</v>
       </c>
       <c r="J31" s="43" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K31" s="27">
         <v>29658</v>
@@ -3865,10 +3859,10 @@
         <v>58</v>
       </c>
       <c r="F32" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H32" s="25" t="s">
         <v>64</v>
@@ -3903,10 +3897,10 @@
         <v>58</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H33" s="25" t="s">
         <v>83</v>
@@ -3941,10 +3935,10 @@
         <v>58</v>
       </c>
       <c r="F34" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H34" s="25" t="s">
         <v>69</v>
@@ -3979,10 +3973,10 @@
         <v>58</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H35" s="25" t="s">
         <v>72</v>
@@ -4017,10 +4011,10 @@
         <v>58</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H36" s="25" t="s">
         <v>72</v>
@@ -4055,7 +4049,7 @@
         <v>58</v>
       </c>
       <c r="F37" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G37" s="31" t="s">
         <v>105</v>
@@ -4093,7 +4087,7 @@
         <v>58</v>
       </c>
       <c r="F38" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G38" s="31" t="s">
         <v>105</v>
@@ -4131,7 +4125,7 @@
         <v>58</v>
       </c>
       <c r="F39" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G39" s="31" t="s">
         <v>105</v>
@@ -4169,7 +4163,7 @@
         <v>58</v>
       </c>
       <c r="F40" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G40" s="31" t="s">
         <v>105</v>
@@ -4207,7 +4201,7 @@
         <v>58</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G41" s="31" t="s">
         <v>105</v>
@@ -4245,7 +4239,7 @@
         <v>58</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G42" s="31" t="s">
         <v>105</v>
@@ -4283,7 +4277,7 @@
         <v>58</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G43" s="31" t="s">
         <v>105</v>
@@ -4321,10 +4315,10 @@
         <v>58</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G44" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H44" s="25" t="s">
         <v>64</v>
@@ -4359,10 +4353,10 @@
         <v>58</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G45" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H45" s="25" t="s">
         <v>83</v>
@@ -4397,10 +4391,10 @@
         <v>58</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G46" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H46" s="25" t="s">
         <v>66</v>
@@ -4435,10 +4429,10 @@
         <v>58</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G47" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H47" s="25" t="s">
         <v>87</v>
@@ -4473,10 +4467,10 @@
         <v>58</v>
       </c>
       <c r="F48" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G48" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H48" s="25" t="s">
         <v>69</v>
@@ -4511,10 +4505,10 @@
         <v>58</v>
       </c>
       <c r="F49" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G49" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H49" s="25" t="s">
         <v>69</v>
@@ -4549,10 +4543,10 @@
         <v>58</v>
       </c>
       <c r="F50" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G50" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H50" s="25" t="s">
         <v>72</v>
@@ -4587,10 +4581,10 @@
         <v>58</v>
       </c>
       <c r="F51" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G51" s="32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H51" s="25" t="s">
         <v>72</v>
@@ -4625,10 +4619,10 @@
         <v>58</v>
       </c>
       <c r="F52" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G52" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H52" s="25" t="s">
         <v>64</v>
@@ -4663,10 +4657,10 @@
         <v>58</v>
       </c>
       <c r="F53" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G53" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H53" s="25" t="s">
         <v>64</v>
@@ -4701,10 +4695,10 @@
         <v>58</v>
       </c>
       <c r="F54" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G54" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H54" s="25" t="s">
         <v>83</v>
@@ -4739,10 +4733,10 @@
         <v>58</v>
       </c>
       <c r="F55" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G55" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H55" s="25" t="s">
         <v>83</v>
@@ -4777,10 +4771,10 @@
         <v>58</v>
       </c>
       <c r="F56" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G56" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H56" s="25" t="s">
         <v>83</v>
@@ -4815,10 +4809,10 @@
         <v>58</v>
       </c>
       <c r="F57" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G57" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H57" s="25" t="s">
         <v>122</v>
@@ -4853,10 +4847,10 @@
         <v>58</v>
       </c>
       <c r="F58" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G58" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H58" s="25" t="s">
         <v>66</v>
@@ -4891,10 +4885,10 @@
         <v>58</v>
       </c>
       <c r="F59" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H59" s="25" t="s">
         <v>87</v>
@@ -4929,10 +4923,10 @@
         <v>58</v>
       </c>
       <c r="F60" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H60" s="25" t="s">
         <v>69</v>
@@ -4967,10 +4961,10 @@
         <v>58</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G61" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H61" s="25" t="s">
         <v>69</v>
@@ -5005,10 +4999,10 @@
         <v>58</v>
       </c>
       <c r="F62" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G62" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H62" s="25" t="s">
         <v>72</v>
@@ -5043,10 +5037,10 @@
         <v>58</v>
       </c>
       <c r="F63" s="41" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H63" s="25" t="s">
         <v>72</v>
@@ -5081,10 +5075,10 @@
         <v>58</v>
       </c>
       <c r="F64" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H64" s="25" t="s">
         <v>64</v>
@@ -5119,10 +5113,10 @@
         <v>58</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H65" s="25" t="s">
         <v>64</v>
@@ -5157,10 +5151,10 @@
         <v>58</v>
       </c>
       <c r="F66" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H66" s="25" t="s">
         <v>83</v>
@@ -5195,10 +5189,10 @@
         <v>58</v>
       </c>
       <c r="F67" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H67" s="25" t="s">
         <v>83</v>
@@ -5233,10 +5227,10 @@
         <v>58</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H68" s="25" t="s">
         <v>122</v>
@@ -5271,10 +5265,10 @@
         <v>58</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H69" s="25" t="s">
         <v>66</v>
@@ -5309,10 +5303,10 @@
         <v>58</v>
       </c>
       <c r="F70" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H70" s="25" t="s">
         <v>87</v>
@@ -5347,10 +5341,10 @@
         <v>58</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H71" s="25" t="s">
         <v>69</v>
@@ -5385,10 +5379,10 @@
         <v>58</v>
       </c>
       <c r="F72" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H72" s="25" t="s">
         <v>69</v>
@@ -5423,10 +5417,10 @@
         <v>58</v>
       </c>
       <c r="F73" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G73" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H73" s="25" t="s">
         <v>72</v>
@@ -5461,10 +5455,10 @@
         <v>58</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G74" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H74" s="25" t="s">
         <v>72</v>
@@ -5499,10 +5493,10 @@
         <v>58</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G75" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H75" s="25" t="s">
         <v>64</v>
@@ -5537,10 +5531,10 @@
         <v>58</v>
       </c>
       <c r="F76" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G76" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H76" s="25" t="s">
         <v>64</v>
@@ -5575,10 +5569,10 @@
         <v>58</v>
       </c>
       <c r="F77" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G77" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H77" s="25" t="s">
         <v>83</v>
@@ -5613,10 +5607,10 @@
         <v>58</v>
       </c>
       <c r="F78" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G78" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H78" s="25" t="s">
         <v>83</v>
@@ -5651,10 +5645,10 @@
         <v>58</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G79" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H79" s="25" t="s">
         <v>122</v>
@@ -5689,10 +5683,10 @@
         <v>58</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G80" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H80" s="25" t="s">
         <v>66</v>
@@ -5727,10 +5721,10 @@
         <v>58</v>
       </c>
       <c r="F81" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G81" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H81" s="25" t="s">
         <v>87</v>
@@ -5765,10 +5759,10 @@
         <v>58</v>
       </c>
       <c r="F82" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G82" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H82" s="25" t="s">
         <v>69</v>
@@ -5803,10 +5797,10 @@
         <v>58</v>
       </c>
       <c r="F83" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G83" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H83" s="25" t="s">
         <v>69</v>
@@ -5841,10 +5835,10 @@
         <v>58</v>
       </c>
       <c r="F84" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G84" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H84" s="25" t="s">
         <v>72</v>
@@ -5879,10 +5873,10 @@
         <v>58</v>
       </c>
       <c r="F85" s="41" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G85" s="35" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H85" s="25" t="s">
         <v>72</v>
@@ -8620,8 +8614,8 @@
   </sheetPr>
   <dimension ref="A1:L906"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8684,25 +8678,25 @@
         <v>139</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>140</v>
+        <v>187</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>59</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K2" s="27">
         <v>35343</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75">
@@ -8722,25 +8716,25 @@
         <v>139</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>59</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J3" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K3" s="27">
         <v>54275</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75">
@@ -11523,31 +11517,31 @@
         <v>12</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="F2" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="G2" s="40" t="s">
+      <c r="I2" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>150</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="K2" s="27">
         <v>10829</v>
@@ -11558,31 +11552,31 @@
         <v>12</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="40" t="s">
         <v>147</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>149</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J3" s="41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K3" s="27">
         <v>9755</v>
@@ -14300,8 +14294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B855F4CF-4650-45D4-87F0-B29B2A97A803}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14314,7 +14308,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -14383,7 +14377,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B10">
         <v>35</v>
@@ -14391,7 +14385,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>35</v>
@@ -14399,7 +14393,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B12">
         <v>35</v>
@@ -14407,7 +14401,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B13">
         <v>35</v>
@@ -14415,7 +14409,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14">
         <v>35</v>
@@ -14431,7 +14425,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B16">
         <v>35</v>
@@ -14439,7 +14433,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B17">
         <v>35</v>
@@ -14447,7 +14441,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B18">
         <v>35</v>
@@ -14455,7 +14449,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B19">
         <v>35</v>
@@ -14463,7 +14457,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B20">
         <v>30</v>
@@ -14471,7 +14465,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B21">
         <v>30</v>
@@ -14479,7 +14473,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B22">
         <v>20</v>

</xml_diff>